<commit_message>
Works and Finance changes
</commit_message>
<xml_diff>
--- a/egov/egov-worksweb/src/main/webapp/resources/app/formats/BOQ_Upload_Format.xlsx
+++ b/egov/egov-worksweb/src/main/webapp/resources/app/formats/BOQ_Upload_Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajatp932\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajatp932\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2F41A0-94F3-4F68-95C2-2DEABBDF1AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED986F6-CF40-4EBE-8094-522C1642D14D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,22 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>item_description</t>
-  </si>
-  <si>
-    <t>ref_dsr</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Test1</t>
   </si>
@@ -56,6 +41,54 @@
   </si>
   <si>
     <t>cm</t>
+  </si>
+  <si>
+    <t>MileStone1</t>
+  </si>
+  <si>
+    <t>MileStone2</t>
+  </si>
+  <si>
+    <t>MileStone3</t>
+  </si>
+  <si>
+    <t>MileStone4</t>
+  </si>
+  <si>
+    <t>Test455</t>
+  </si>
+  <si>
+    <t>Test3 Desc gou</t>
+  </si>
+  <si>
+    <t>Test456</t>
+  </si>
+  <si>
+    <t>MileStone5</t>
+  </si>
+  <si>
+    <t>Test457</t>
+  </si>
+  <si>
+    <t>Test458</t>
+  </si>
+  <si>
+    <t>Scope/Milestone</t>
+  </si>
+  <si>
+    <t>Ref DSR/NS</t>
+  </si>
+  <si>
+    <t>Item Description</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -105,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -128,17 +161,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,90 +431,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="26" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="27" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F2" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
         <v>3</v>
       </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4</v>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1416,8 +1588,6 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>